<commit_message>
fix academic offer update
</commit_message>
<xml_diff>
--- a/data/universidades.xlsx
+++ b/data/universidades.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/boris/Sites/gape/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elcoruco/Sites/gape/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="29220" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="1900" yWindow="10920" windowWidth="29220" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="140">
   <si>
     <t>universidad</t>
   </si>
@@ -269,9 +269,6 @@
     <t>http://www.upamozoc.edu.mx</t>
   </si>
   <si>
-    <t>Universidad Politécnica de Amozoc</t>
-  </si>
-  <si>
     <t>(222) 168 85 67</t>
   </si>
   <si>
@@ -429,6 +426,24 @@
   </si>
   <si>
     <t>Hugo Osorio</t>
+  </si>
+  <si>
+    <t>Universidad Politécnica de Amozoc de Mota</t>
+  </si>
+  <si>
+    <t>Instituto Tecnológico Superior de la Sierra Norte de Puebla</t>
+  </si>
+  <si>
+    <t>http://www.itssnp.edu.mx/v2/</t>
+  </si>
+  <si>
+    <t>Zacatlán</t>
+  </si>
+  <si>
+    <t>797 975 16 94</t>
+  </si>
+  <si>
+    <t>Av. José Luis Martínez Vázquez No. 2000. Jicolapa, Zacatlán, Pue</t>
   </si>
 </sst>
 </file>
@@ -754,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1121,22 +1136,22 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
         <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" t="s">
         <v>82</v>
-      </c>
-      <c r="F17" t="s">
-        <v>83</v>
       </c>
       <c r="G17">
         <v>72980</v>
@@ -1144,22 +1159,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" t="s">
         <v>86</v>
       </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
         <v>87</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F18" t="s">
-        <v>88</v>
       </c>
       <c r="G18">
         <v>74420</v>
@@ -1167,22 +1182,22 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
         <v>91</v>
       </c>
-      <c r="B19" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" t="s">
         <v>92</v>
-      </c>
-      <c r="D19" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" t="s">
-        <v>93</v>
       </c>
       <c r="G19">
         <v>75020</v>
@@ -1190,22 +1205,22 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" t="s">
         <v>97</v>
-      </c>
-      <c r="D20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" t="s">
-        <v>98</v>
       </c>
       <c r="G20">
         <v>75859</v>
@@ -1213,19 +1228,19 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
         <v>101</v>
       </c>
-      <c r="B21" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
         <v>102</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" t="s">
-        <v>103</v>
       </c>
       <c r="G21">
         <v>73080</v>
@@ -1233,13 +1248,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
         <v>104</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
@@ -1247,22 +1262,22 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
         <v>107</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" t="s">
-        <v>108</v>
       </c>
       <c r="G23">
         <v>74169</v>
@@ -1270,22 +1285,22 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" t="s">
         <v>112</v>
-      </c>
-      <c r="B24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s">
-        <v>114</v>
-      </c>
-      <c r="F24" t="s">
-        <v>113</v>
       </c>
       <c r="G24">
         <v>72300</v>
@@ -1293,22 +1308,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>119</v>
+      </c>
+      <c r="F25" t="s">
         <v>117</v>
-      </c>
-      <c r="B25" t="s">
-        <v>116</v>
-      </c>
-      <c r="C25" t="s">
-        <v>119</v>
-      </c>
-      <c r="D25" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s">
-        <v>120</v>
-      </c>
-      <c r="F25" t="s">
-        <v>118</v>
       </c>
       <c r="G25">
         <v>73475</v>
@@ -1316,22 +1331,22 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
+        <v>124</v>
+      </c>
+      <c r="F26" t="s">
         <v>123</v>
-      </c>
-      <c r="D26" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s">
-        <v>125</v>
-      </c>
-      <c r="F26" t="s">
-        <v>124</v>
       </c>
       <c r="G26">
         <v>74949</v>
@@ -1339,42 +1354,62 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" t="s">
         <v>127</v>
-      </c>
-      <c r="B27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
         <v>131</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" t="s">
         <v>133</v>
       </c>
-      <c r="I28" t="s">
-        <v>134</v>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>